<commit_message>
learning (my app with registration login mysql download uploads excel works) I have added a function which check what extension file and if this is a xlsx - it will convert this file to csv
</commit_message>
<xml_diff>
--- a/downloads/newDataFile.xlsx
+++ b/downloads/newDataFile.xlsx
@@ -10,10 +10,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -44,10 +42,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,116 +375,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <v>Region</v>
-      </c>
-      <c r="C1" s="1" t="str">
-        <v>Brand</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <v>State</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <v>Net</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>42133</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <v>May</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <v>ADIDAS</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <v>NY</v>
-      </c>
-      <c r="E2" s="1">
-        <v>13.559999999999999</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2">
-        <v>42509</v>
-      </c>
-      <c r="B3" s="1" t="str">
-        <v>June</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <v>NEW BALANCE</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <v>IL</v>
-      </c>
-      <c r="E3" s="1">
-        <v>10.38</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>42742</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <v>July</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <v>TOMMY HILFIGER</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <v>OH</v>
-      </c>
-      <c r="E4" s="1">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>42489</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <v>August</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <v>M TAC</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <v>NV</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-203</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>42974</v>
-      </c>
-      <c r="B6" s="1" t="str">
-        <v>September</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5.11</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <v>CA</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-206</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>